<commit_message>
Fixed Third Party timelines and error in Tyler labelling
</commit_message>
<xml_diff>
--- a/Presidential Timeline.xlsx
+++ b/Presidential Timeline.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a65e975236fa3b36/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\khora\Documents\GitHub\APUSH-Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{55C5D72E-8E1C-4560-BE9A-1D1479584D58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C1E8DC6D-FE6C-4227-A56A-E40D2B86643C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D2F04F-6032-454B-98EE-397F736850BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ED6EDC44-F4A8-46AA-B4C9-693CA238D22E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Term</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>Anti-Masonic</t>
+  </si>
+  <si>
+    <t>Constitutional Union</t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +293,16 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <gradientFill>
+        <stop position="0">
+          <color rgb="FFFF66FF"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF6464FF"/>
+        </stop>
+      </gradientFill>
+    </fill>
   </fills>
   <borders count="52">
     <border>
@@ -956,64 +969,88 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1024,6 +1061,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1033,18 +1079,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1054,272 +1088,275 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1329,9 +1366,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FF00FF99"/>
       <color rgb="FF6464FF"/>
       <color rgb="FFFF66FF"/>
+      <color rgb="FF00FF99"/>
       <color rgb="FFFF6464"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFD77DFF"/>
@@ -1647,10 +1684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0533EE4-0E4C-457B-A0B9-30036464F7A8}">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17:L20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,876 +1699,895 @@
     <col min="5" max="5" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="14" width="7.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="23" t="s">
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="2" t="s">
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="117" t="s">
+      <c r="T1" s="22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="30" t="s">
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31" t="s">
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="118"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="23"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="36">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>1789</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="3">
         <f>A3+1</f>
         <v>1790</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="4">
         <f>B3+4</f>
         <v>1794</v>
       </c>
-      <c r="D3" s="39">
+      <c r="D3" s="31">
         <v>1</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="41"/>
-      <c r="G3" s="24" t="s">
+      <c r="F3" s="97"/>
+      <c r="G3" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="2" t="s">
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="S3" s="117" t="s">
+      <c r="T3" s="22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="43">
+    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="115">
         <v>1792</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="116">
         <f t="shared" ref="B4:B24" si="0">A4+1</f>
         <v>1793</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="117">
         <f t="shared" ref="C4:C24" si="1">B4+4</f>
         <v>1797</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="119"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="27"/>
     </row>
-    <row r="5" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="43">
+    <row r="5" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="115">
         <f>A4+4</f>
         <v>1796</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="116">
         <f t="shared" si="0"/>
         <v>1797</v>
       </c>
-      <c r="C5" s="45">
+      <c r="C5" s="117">
         <f t="shared" si="1"/>
         <v>1801</v>
       </c>
-      <c r="D5" s="49">
+      <c r="D5" s="10">
         <v>2</v>
       </c>
-      <c r="E5" s="50" t="s">
+      <c r="E5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="51"/>
-      <c r="G5" s="13" t="s">
+      <c r="F5" s="12"/>
+      <c r="G5" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="52" t="s">
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="42"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="118"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="100"/>
+      <c r="N5" s="101"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="23"/>
     </row>
-    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43">
-        <f t="shared" ref="A6:A24" si="2">A5+4</f>
+    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="115">
+        <f t="shared" ref="A6:A45" si="2">A5+4</f>
         <v>1800</v>
       </c>
-      <c r="B6" s="44">
+      <c r="B6" s="116">
         <f t="shared" si="0"/>
         <v>1801</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="117">
         <f t="shared" si="1"/>
         <v>1805</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="32">
         <v>3</v>
       </c>
-      <c r="E6" s="55" t="s">
+      <c r="E6" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="48"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="2" t="s">
+      <c r="F6" s="98"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="103"/>
+      <c r="M6" s="103"/>
+      <c r="N6" s="104"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="43">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="115">
         <f t="shared" si="2"/>
         <v>1804</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="116">
         <f t="shared" si="0"/>
         <v>1805</v>
       </c>
-      <c r="C7" s="45">
+      <c r="C7" s="117">
         <f t="shared" si="1"/>
         <v>1809</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="57"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="42"/>
-      <c r="P7" s="42"/>
-      <c r="Q7" s="42"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="102"/>
+      <c r="L7" s="103"/>
+      <c r="M7" s="103"/>
+      <c r="N7" s="104"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="43">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="115">
         <f t="shared" si="2"/>
         <v>1808</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="116">
         <f t="shared" si="0"/>
         <v>1809</v>
       </c>
-      <c r="C8" s="45">
+      <c r="C8" s="117">
         <f t="shared" si="1"/>
         <v>1813</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="32">
         <v>4</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="48"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="57"/>
-      <c r="M8" s="57"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="29"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="103"/>
+      <c r="M8" s="103"/>
+      <c r="N8" s="104"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
     </row>
-    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="43">
+    <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="115">
         <f t="shared" si="2"/>
         <v>1812</v>
       </c>
-      <c r="B9" s="44">
+      <c r="B9" s="116">
         <f t="shared" si="0"/>
         <v>1813</v>
       </c>
-      <c r="C9" s="45">
+      <c r="C9" s="117">
         <f t="shared" si="1"/>
         <v>1817</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="61"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="42"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="98"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="106"/>
+      <c r="M9" s="106"/>
+      <c r="N9" s="107"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="43">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="115">
         <f t="shared" si="2"/>
         <v>1816</v>
       </c>
-      <c r="B10" s="44">
+      <c r="B10" s="116">
         <f t="shared" si="0"/>
         <v>1817</v>
       </c>
-      <c r="C10" s="45">
+      <c r="C10" s="117">
         <f t="shared" si="1"/>
         <v>1821</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="32">
         <v>5</v>
       </c>
-      <c r="E10" s="62" t="s">
+      <c r="E10" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="48"/>
-      <c r="G10" s="63" t="s">
+      <c r="F10" s="98"/>
+      <c r="G10" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="63"/>
-      <c r="L10" s="63"/>
-      <c r="M10" s="63"/>
-      <c r="N10" s="64"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="61"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="43">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="115">
         <f t="shared" si="2"/>
         <v>1820</v>
       </c>
-      <c r="B11" s="44">
+      <c r="B11" s="116">
         <f t="shared" si="0"/>
         <v>1821</v>
       </c>
-      <c r="C11" s="45">
+      <c r="C11" s="117">
         <f t="shared" si="1"/>
         <v>1825</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="64"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="29"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="61"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
     </row>
-    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="43">
+    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="115">
         <f t="shared" si="2"/>
         <v>1824</v>
       </c>
-      <c r="B12" s="44">
+      <c r="B12" s="116">
         <f t="shared" si="0"/>
         <v>1825</v>
       </c>
-      <c r="C12" s="45">
+      <c r="C12" s="117">
         <f t="shared" si="1"/>
         <v>1829</v>
       </c>
-      <c r="D12" s="49">
+      <c r="D12" s="10">
         <v>6</v>
       </c>
-      <c r="E12" s="65" t="s">
+      <c r="E12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="51"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="29"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="62"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="26"/>
+      <c r="T12" s="25"/>
     </row>
-    <row r="13" spans="1:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="43">
+    <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="115">
         <f t="shared" si="2"/>
         <v>1828</v>
       </c>
-      <c r="B13" s="44">
+      <c r="B13" s="116">
         <f t="shared" si="0"/>
         <v>1829</v>
       </c>
-      <c r="C13" s="45">
+      <c r="C13" s="117">
         <f t="shared" si="1"/>
         <v>1833</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="32">
         <v>7</v>
       </c>
-      <c r="E13" s="68" t="s">
+      <c r="E13" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="48"/>
-      <c r="G13" s="69" t="s">
+      <c r="F13" s="98"/>
+      <c r="G13" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="70"/>
-      <c r="I13" s="70"/>
-      <c r="J13" s="71"/>
-      <c r="K13" s="72" t="s">
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="111" t="s">
         <v>47</v>
       </c>
-      <c r="L13" s="73"/>
-      <c r="M13" s="73"/>
-      <c r="N13" s="74"/>
-      <c r="O13" s="121" t="s">
+      <c r="L13" s="112"/>
+      <c r="M13" s="112"/>
+      <c r="N13" s="113"/>
+      <c r="O13" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="2" t="s">
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="S13" s="29"/>
+      <c r="T13" s="25"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="43">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="115">
         <f t="shared" si="2"/>
         <v>1832</v>
       </c>
-      <c r="B14" s="44">
+      <c r="B14" s="116">
         <f t="shared" si="0"/>
         <v>1833</v>
       </c>
-      <c r="C14" s="45">
+      <c r="C14" s="117">
         <f t="shared" si="1"/>
         <v>1837</v>
       </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="78" t="s">
+      <c r="D14" s="32"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="L14" s="79"/>
-      <c r="M14" s="79"/>
-      <c r="N14" s="80"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="29"/>
-      <c r="S14" s="29"/>
+      <c r="L14" s="109"/>
+      <c r="M14" s="109"/>
+      <c r="N14" s="110"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="25"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="43">
+    <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="115">
         <f t="shared" si="2"/>
         <v>1836</v>
       </c>
-      <c r="B15" s="44">
+      <c r="B15" s="116">
         <f t="shared" si="0"/>
         <v>1837</v>
       </c>
-      <c r="C15" s="45">
+      <c r="C15" s="117">
         <f t="shared" si="1"/>
         <v>1841</v>
       </c>
-      <c r="D15" s="49">
+      <c r="D15" s="10">
         <v>8</v>
       </c>
-      <c r="E15" s="81" t="s">
+      <c r="E15" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="82"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="76"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="80"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="29"/>
-      <c r="S15" s="29"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="108"/>
+      <c r="L15" s="109"/>
+      <c r="M15" s="109"/>
+      <c r="N15" s="110"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="43">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="115">
         <f t="shared" si="2"/>
         <v>1840</v>
       </c>
-      <c r="B16" s="44">
+      <c r="B16" s="116">
         <f t="shared" si="0"/>
         <v>1841</v>
       </c>
-      <c r="C16" s="45">
+      <c r="C16" s="117">
         <f t="shared" si="1"/>
         <v>1845</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="83" t="s">
+      <c r="E16" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="84" t="s">
+      <c r="F16" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="75"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="77"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="79"/>
-      <c r="M16" s="79"/>
-      <c r="N16" s="80"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="29"/>
-      <c r="S16" s="29"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="108"/>
+      <c r="L16" s="109"/>
+      <c r="M16" s="109"/>
+      <c r="N16" s="110"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="122" t="s">
+        <v>39</v>
+      </c>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="43">
+    <row r="17" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="115">
         <f t="shared" si="2"/>
         <v>1844</v>
       </c>
-      <c r="B17" s="44">
+      <c r="B17" s="116">
         <f t="shared" si="0"/>
         <v>1845</v>
       </c>
-      <c r="C17" s="45">
+      <c r="C17" s="117">
         <f t="shared" si="1"/>
         <v>1849</v>
       </c>
-      <c r="D17" s="49">
+      <c r="D17" s="10">
         <v>11</v>
       </c>
-      <c r="E17" s="85" t="s">
+      <c r="E17" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="76"/>
-      <c r="J17" s="77"/>
-      <c r="K17" s="4" t="s">
+      <c r="F17" s="9"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="L17" s="5"/>
-      <c r="M17" s="86" t="s">
-        <v>38</v>
-      </c>
-      <c r="N17" s="87"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="29"/>
-      <c r="S17" s="29"/>
+      <c r="L17" s="75"/>
+      <c r="M17" s="80"/>
+      <c r="N17" s="81"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="123"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
     </row>
-    <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="43">
+    <row r="18" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="115">
         <f t="shared" si="2"/>
         <v>1848</v>
       </c>
-      <c r="B18" s="44">
+      <c r="B18" s="116">
         <f t="shared" si="0"/>
         <v>1849</v>
       </c>
-      <c r="C18" s="45">
+      <c r="C18" s="117">
         <f t="shared" si="1"/>
         <v>1853</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="83" t="s">
+      <c r="E18" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="88" t="s">
+      <c r="F18" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="75"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="76"/>
-      <c r="J18" s="77"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="89"/>
-      <c r="N18" s="90"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="3"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="76"/>
+      <c r="L18" s="77"/>
+      <c r="M18" s="82"/>
+      <c r="N18" s="83"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="125" t="s">
+        <v>41</v>
+      </c>
+      <c r="R18" s="124"/>
+      <c r="S18" s="25"/>
+      <c r="T18" s="26"/>
     </row>
-    <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="43">
+    <row r="19" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="115">
         <f t="shared" si="2"/>
         <v>1852</v>
       </c>
-      <c r="B19" s="44">
+      <c r="B19" s="116">
         <f t="shared" si="0"/>
         <v>1853</v>
       </c>
-      <c r="C19" s="45">
+      <c r="C19" s="117">
         <f t="shared" si="1"/>
         <v>1857</v>
       </c>
-      <c r="D19" s="49">
+      <c r="D19" s="10">
         <v>14</v>
       </c>
-      <c r="E19" s="81" t="s">
+      <c r="E19" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="91"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="76"/>
-      <c r="I19" s="76"/>
-      <c r="J19" s="77"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="89"/>
-      <c r="N19" s="90"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="120" t="s">
+      <c r="F19" s="19"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="76"/>
+      <c r="L19" s="77"/>
+      <c r="M19" s="82"/>
+      <c r="N19" s="83"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="125" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q19" s="123"/>
+      <c r="R19" s="128"/>
+      <c r="S19" s="25"/>
+      <c r="T19" s="20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="43">
+    <row r="20" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="115">
         <f t="shared" si="2"/>
         <v>1856</v>
       </c>
-      <c r="B20" s="44">
+      <c r="B20" s="116">
         <f t="shared" si="0"/>
         <v>1857</v>
       </c>
-      <c r="C20" s="45">
+      <c r="C20" s="117">
         <f t="shared" si="1"/>
         <v>1861</v>
       </c>
-      <c r="D20" s="49">
+      <c r="D20" s="10">
         <v>15</v>
       </c>
-      <c r="E20" s="81" t="s">
+      <c r="E20" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="82"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="76"/>
-      <c r="J20" s="77"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="92"/>
-      <c r="N20" s="93"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="2" t="s">
+      <c r="F20" s="15"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="78"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="84"/>
+      <c r="N20" s="85"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="126"/>
+      <c r="Q20" s="123"/>
+      <c r="R20" s="128"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="24" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="43">
+    <row r="21" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="115">
         <f t="shared" si="2"/>
         <v>1860</v>
       </c>
-      <c r="B21" s="44">
+      <c r="B21" s="116">
         <f t="shared" si="0"/>
         <v>1861</v>
       </c>
-      <c r="C21" s="45">
+      <c r="C21" s="117">
         <f t="shared" si="1"/>
         <v>1865</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="94" t="s">
+      <c r="E21" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="95" t="s">
+      <c r="F21" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11" t="s">
+      <c r="H21" s="52"/>
+      <c r="I21" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="J21" s="12"/>
-      <c r="K21" s="96" t="s">
+      <c r="J21" s="53"/>
+      <c r="K21" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="L21" s="97"/>
-      <c r="M21" s="97"/>
-      <c r="N21" s="98"/>
-      <c r="O21" s="99" t="s">
-        <v>39</v>
-      </c>
-      <c r="P21" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q21" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="R21" s="2" t="s">
+      <c r="L21" s="87"/>
+      <c r="M21" s="87"/>
+      <c r="N21" s="88"/>
+      <c r="O21" s="121" t="s">
+        <v>57</v>
+      </c>
+      <c r="P21" s="127"/>
+      <c r="Q21" s="124"/>
+      <c r="R21" s="129"/>
+      <c r="S21" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="S21" s="29"/>
+      <c r="T21" s="25"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="43">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="115">
         <f t="shared" si="2"/>
         <v>1864</v>
       </c>
-      <c r="B22" s="44">
+      <c r="B22" s="116">
         <f t="shared" si="0"/>
         <v>1865</v>
       </c>
-      <c r="C22" s="45">
+      <c r="C22" s="117">
         <f t="shared" si="1"/>
         <v>1869</v>
       </c>
-      <c r="D22" s="46"/>
-      <c r="E22" s="94"/>
-      <c r="F22" s="100"/>
-      <c r="G22" s="75" t="s">
+      <c r="D22" s="32"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="76"/>
-      <c r="I22" s="76"/>
-      <c r="J22" s="77"/>
-      <c r="K22" s="101"/>
-      <c r="L22" s="102"/>
-      <c r="M22" s="102"/>
-      <c r="N22" s="103"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="29"/>
-      <c r="S22" s="2" t="s">
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="89"/>
+      <c r="L22" s="90"/>
+      <c r="M22" s="90"/>
+      <c r="N22" s="91"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="25"/>
+      <c r="T22" s="24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="43">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="115">
         <f t="shared" si="2"/>
         <v>1868</v>
       </c>
-      <c r="B23" s="44">
+      <c r="B23" s="116">
         <f t="shared" si="0"/>
         <v>1869</v>
       </c>
-      <c r="C23" s="45">
+      <c r="C23" s="117">
         <f t="shared" si="1"/>
         <v>1873</v>
       </c>
-      <c r="D23" s="46">
+      <c r="D23" s="32">
         <v>18</v>
       </c>
-      <c r="E23" s="94" t="s">
+      <c r="E23" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="104"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="76"/>
-      <c r="I23" s="76"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="101"/>
-      <c r="L23" s="102"/>
-      <c r="M23" s="102"/>
-      <c r="N23" s="103"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="42"/>
-      <c r="Q23" s="42"/>
-      <c r="R23" s="29"/>
-      <c r="S23" s="29"/>
+      <c r="F23" s="95"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="89"/>
+      <c r="L23" s="90"/>
+      <c r="M23" s="90"/>
+      <c r="N23" s="91"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="25"/>
+      <c r="T23" s="25"/>
     </row>
-    <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="105">
+    <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="118">
         <f t="shared" si="2"/>
         <v>1872</v>
       </c>
-      <c r="B24" s="106">
+      <c r="B24" s="119">
         <f t="shared" si="0"/>
         <v>1873</v>
       </c>
-      <c r="C24" s="107">
+      <c r="C24" s="120">
         <f t="shared" si="1"/>
         <v>1877</v>
       </c>
-      <c r="D24" s="108"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="110"/>
-      <c r="G24" s="111"/>
-      <c r="H24" s="112"/>
-      <c r="I24" s="112"/>
-      <c r="J24" s="113"/>
-      <c r="K24" s="114"/>
-      <c r="L24" s="115"/>
-      <c r="M24" s="115"/>
-      <c r="N24" s="116"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="96"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="92"/>
+      <c r="L24" s="93"/>
+      <c r="M24" s="93"/>
+      <c r="N24" s="94"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
+  <mergeCells count="54">
     <mergeCell ref="S1:S2"/>
-    <mergeCell ref="S6:S18"/>
-    <mergeCell ref="S3:S5"/>
-    <mergeCell ref="S20:S21"/>
-    <mergeCell ref="S22:S24"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="G1:N1"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="G3:N4"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="O1:Q2"/>
+    <mergeCell ref="S3:S12"/>
+    <mergeCell ref="S13:S20"/>
+    <mergeCell ref="P19:P21"/>
+    <mergeCell ref="Q18:Q21"/>
+    <mergeCell ref="R16:R18"/>
+    <mergeCell ref="S21:S24"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="K5:N9"/>
+    <mergeCell ref="K14:N16"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="O1:R2"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="E6:E7"/>
@@ -2544,24 +2600,32 @@
     <mergeCell ref="G13:J20"/>
     <mergeCell ref="G10:N12"/>
     <mergeCell ref="G5:J9"/>
-    <mergeCell ref="E23:E24"/>
     <mergeCell ref="G22:J24"/>
     <mergeCell ref="K17:L20"/>
     <mergeCell ref="M17:N20"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="G1:N1"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="G3:N4"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="E23:E24"/>
     <mergeCell ref="K21:N24"/>
     <mergeCell ref="F23:F24"/>
-    <mergeCell ref="R21:R24"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="K5:N9"/>
-    <mergeCell ref="K14:N16"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="R3:R12"/>
-    <mergeCell ref="R13:R20"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="T6:T18"/>
+    <mergeCell ref="T3:T5"/>
+    <mergeCell ref="T20:T21"/>
+    <mergeCell ref="T22:T24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>